<commit_message>
- 3. hét/1. rész
</commit_message>
<xml_diff>
--- a/Dokumentációk/Esemény napló/Chat dokumentálás.xlsx
+++ b/Dokumentációk/Esemény napló/Chat dokumentálás.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Archived\LegyenÖnIsMilliomosProject\Legyen ön is milliomos - Project - UNIDUNA\Dokumentumok\Project kommunikáció előzmények\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Archived\LegyenÖnIsMilliomosProject\Git\Miliomos_Project\Dokumentációk\Esemény napló\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1FF5A1D-1255-41F1-A650-5AE25E7D1C07}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6DC663-5AA3-4466-A1DC-4375A2BEFE89}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Dátum</t>
   </si>
@@ -121,6 +121,9 @@
     </r>
   </si>
   <si>
+    <t>https://dl.dropboxusercontent.com/s/r0x52ape6ghnt8h/chrome_ZJDwQiUWSu.png</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -136,7 +139,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
       </rPr>
-      <t xml:space="preserve"> Project megszervezése, Ideiglenes Facebook csoport megbeszélésekre, Online "raktár" repository létrehozása(GIT), Elvállalt feladatok megszervezése, Management - Nagy Ádám // Front és back-end felkészülések, hivatkozások alapján tanulás - Bajnok Tamás + Tóth Tamás + Varsa Laci // Chat és megbeszélések dokumentálása, ideiglenesen google docs segítségével - Szabó Attila // Regisztráció + Login alap elkezdése - Bajnok Tamás</t>
+      <t xml:space="preserve"> Project megszervezése, Ideiglenes Facebook csoport megbeszélésekre, Online "raktár" repository létrehozása(GIT) / Elvállalt feladatok megszervezése/ Management - Nagy Ádám // Front és back-end felkészülések, hivatkozások alapján tanulás - Bajnok Tamás + Tóth Tamás + Varsa Laci // Chat és megbeszélések dokumentálása, ideiglenesen google docs segítségével - Szabó Attila // Regisztráció + Login alap elkezdése - Bajnok Tamás // Design teszt gráf (melléklet 1.) - Varsa Laci</t>
     </r>
   </si>
   <si>
@@ -148,6 +151,98 @@
         <family val="2"/>
         <charset val="238"/>
       </rPr>
+      <t>Egyéb megjegyzések</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>: 5. hétre működő alap, CSS / back/front-end működjön alapjaiban.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Keddi személyes összejövetel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>: Tanárnővel konzultálás/kérdések, Back-end és front-end áttekintése, Visual Studio, eddigi login alapok tesztelése és demonstrálása - Nagy Ádám, Bajnok Tamás, Front-end-el kapcsolatos tudnivalók átbeszélése és tanulni valók/tervek - Szabó Attila, Varsa Laci, Adatbázisal kapcsolatos tudnivalók és tervek - Tóth Tamás.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve"> Cél megszabása</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>: A program 5.hétre működő képes alapjai meglegyenek, CSS és back/front-end részek alapjaiban működjenek.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Online:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Működő server oldali lekérdezés / login demonstrálása több serverről. - Nagy Ádám, Bajnok Tamás</t>
+    </r>
+  </si>
+  <si>
+    <t>https://dl.dropboxusercontent.com/s/08gsh8gyt3vk8a0/chrome_I44cO1ndDG.png</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
       <t>Szombati összejövetel</t>
     </r>
     <r>
@@ -157,7 +252,7 @@
         <family val="2"/>
         <charset val="238"/>
       </rPr>
-      <t>: Első megbeszélés.</t>
+      <t>: 11:00-kor Online.</t>
     </r>
   </si>
   <si>
@@ -169,6 +264,27 @@
         <family val="2"/>
         <charset val="238"/>
       </rPr>
+      <t>Szombati összejövetel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>: 11:00-kor Online: Első megbeszélés. Csapat név eldöntése. Adatbázis terv excel létrehozása (git-re feltöltése) - Tóth Tamás, Chat dokumentálása/Git használat dokumentálásának elkezdése - Szabó Attila, Git-elérés biztosítása és alapok feltöltése - Nagy Ádám</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
       <t>Egyéb megjegyzések</t>
     </r>
     <r>
@@ -178,7 +294,7 @@
         <family val="2"/>
         <charset val="238"/>
       </rPr>
-      <t>: Nincs</t>
+      <t>: Következő személyes megbeszélésen back-end és front-end alapjainak megbeszélése. Probléma elkerülése érdekében a program felépítésének áttekintése (verzió kezelés).</t>
     </r>
   </si>
 </sst>
@@ -186,7 +302,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -214,6 +330,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="5">
@@ -368,10 +490,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -382,68 +505,75 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hivatkozás" xfId="1" builtinId="8"/>
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -759,10 +889,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:E15"/>
+  <dimension ref="B1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -776,158 +906,192 @@
   <sheetData>
     <row r="1" spans="2:5" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="15" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="18"/>
+      <c r="E3" s="11"/>
     </row>
     <row r="4" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="6"/>
     </row>
     <row r="5" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="14" t="s">
+      <c r="B5" s="18"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="9"/>
+      <c r="E5" s="25" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="9"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="2:5" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="12" t="s">
+      <c r="B7" s="19"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="24"/>
+    </row>
+    <row r="8" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="18"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="18"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="2:5" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="19"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="3"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="3"/>
     </row>
+    <row r="16" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="C4:C7"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C8:C11"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{0C6D9F65-035A-46DB-BD55-C1313CA33086}"/>
+    <hyperlink ref="E5" r:id="rId2" xr:uid="{DFAAE7C7-9BD2-43F8-BD93-C95F32B8D375}"/>
+    <hyperlink ref="E8" r:id="rId3" xr:uid="{EA3C2F54-E0E3-4945-B052-D12A66D9CA56}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Dokumentálás frissítése, commit test új local git mappából.
</commit_message>
<xml_diff>
--- a/Dokumentációk/Esemény napló/Chat dokumentálás.xlsx
+++ b/Dokumentációk/Esemény napló/Chat dokumentálás.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Archived\LegyenÖnIsMilliomosProject\Git\Miliomos_Project\Dokumentációk\Esemény napló\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Szabó Attila\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF7A940-7421-4A15-9CD4-D649DC2B6890}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3D1767-8FC6-4B84-B36B-D80ED098CFA0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -143,6 +143,30 @@
     </r>
   </si>
   <si>
+    <t>https://dl.dropboxusercontent.com/s/08gsh8gyt3vk8a0/chrome_I44cO1ndDG.png</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Szombati összejövetel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>: 11:00-kor Online: Első megbeszélés. Csapat név eldöntése. Adatbázis terv excel létrehozása (git-re feltöltése) - Tóth Tamás, Chat dokumentálása/Git használat dokumentálásának elkezdése - Szabó Attila, Git-elérés biztosítása és alapok feltöltése - Nagy Ádám</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -160,7 +184,18 @@
         <family val="2"/>
         <charset val="238"/>
       </rPr>
-      <t>: 5. hétre működő alap, CSS / back/front-end működjön alapjaiban.</t>
+      <t xml:space="preserve">: Következő személyes megbeszélésen back-end és front-end alapjainak megbeszélése. Probléma elkerülése érdekében a program felépítésének áttekintése (verzió kezelés). </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Határidőn belül elküldeni a tanárnőnek a beadandó dokumentumot (nevek/választott project)</t>
     </r>
   </si>
   <si>
@@ -200,7 +235,50 @@
         <family val="2"/>
         <charset val="238"/>
       </rPr>
-      <t>: A program 5.hétre működő képes alapjai meglegyenek, CSS és back/front-end részek alapjaiban működjenek.</t>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>A program 5.hétre működő képes alapjai meglegyenek, CSS és back/front-end részek alapjaiban működjenek.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Egyéb megjegyzések</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>5. hétre működő alap, CSS / back/front-end működjön alapjaiban.</t>
     </r>
   </si>
   <si>
@@ -228,84 +306,48 @@
         <family val="2"/>
         <charset val="238"/>
       </rPr>
-      <t>Működő server oldali lekérdezés / login demonstrálása több serverről. - Nagy Ádám, Bajnok Tamás</t>
-    </r>
-  </si>
-  <si>
-    <t>https://dl.dropboxusercontent.com/s/08gsh8gyt3vk8a0/chrome_I44cO1ndDG.png</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>Szombati összejövetel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>: 11:00-kor Online.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>Szombati összejövetel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>: 11:00-kor Online: Első megbeszélés. Csapat név eldöntése. Adatbázis terv excel létrehozása (git-re feltöltése) - Tóth Tamás, Chat dokumentálása/Git használat dokumentálásának elkezdése - Szabó Attila, Git-elérés biztosítása és alapok feltöltése - Nagy Ádám</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>Egyéb megjegyzések</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve">: Következő személyes megbeszélésen back-end és front-end alapjainak megbeszélése. Probléma elkerülése érdekében a program felépítésének áttekintése (verzió kezelés). </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>Határidőn belül elküldeni a tanárnőnek a beadandó dokumentumot (nevek/választott project)</t>
+      <t xml:space="preserve">Működő server oldali lekérdezés / login demonstrálása több serverről. - Nagy Ádám, Bajnok Tamás,  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Szerda</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>: Cordova alapok átalakításának tevezése - Nagy Ádám, Vizuális külalak / színek tervezésének elkezdése - Varsa Laci, Képszerkesztő program előkészítése, háttérhez (menü)-höz való készületek (lehetséges hogy 3D-ből 2D-s kép készítése) - Szabó Attila</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>összejövetel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>: ETA</t>
     </r>
   </si>
 </sst>
@@ -313,7 +355,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -356,6 +398,22 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF7030A0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -514,7 +572,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="26">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -524,16 +582,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -560,8 +618,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -575,20 +642,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -910,8 +968,8 @@
   </sheetPr>
   <dimension ref="B1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -951,80 +1009,80 @@
       <c r="E3" s="11"/>
     </row>
     <row r="4" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="23" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="17" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="18"/>
-      <c r="C5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="24"/>
       <c r="D5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="19" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="18"/>
-      <c r="C6" s="21"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="24"/>
       <c r="D6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="2:5" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="22"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="18"/>
+    </row>
+    <row r="8" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="2:5" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="19"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="5" t="s">
+      <c r="E8" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="21"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="21"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="24"/>
-    </row>
-    <row r="8" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="18"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="18"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="7" t="s">
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="2:5" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="22"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="2:5" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="19"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="E11" s="6"/>
     </row>

</xml_diff>

<commit_message>
- 3. Hét dokumentálás, part 1.
</commit_message>
<xml_diff>
--- a/Dokumentációk/Esemény napló/Chat dokumentálás.xlsx
+++ b/Dokumentációk/Esemény napló/Chat dokumentálás.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Szabó Attila\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Archived\MilliomosProject\Miliomos_Project\Dokumentációk\Esemény napló\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3D1767-8FC6-4B84-B36B-D80ED098CFA0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6C9A5A-7014-4CDE-BB59-4A936529C7F4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Dátum</t>
   </si>
@@ -338,7 +338,47 @@
         <family val="2"/>
         <charset val="238"/>
       </rPr>
-      <t>összejövetel</t>
+      <t>Összejövetel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>: Közös megeggyezés alapján áttéve jövőhétre. Egyenlőre mindenki Online haladt a saját részének tanulásával (back-end/front-end)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Online:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Online összejövetel</t>
     </r>
     <r>
       <rPr>
@@ -348,6 +388,107 @@
         <charset val="238"/>
       </rPr>
       <t>: ETA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Egyéb megjegyzések</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Front-end, CSS rész működjön jövőhétre!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve"> 5. Hétre működjön V1 verzió: alapok, működő játék + kinézet! Később ki lesz még egészítve.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Keddi személyes összejövetel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">: Tanóra után: Back-end és Front-end demonstrálása, Cornova rendszerbe belevonni Bajnok Tamás HTML részét (div form megjelenés, 1 indexbe lévő alap), </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>sikeres lefuttatás</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>, mobilon keresztül developer mode(fejlesztői mód) használata,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve"> játék tesztelése közösen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>. - Bajnok Tamás, Nagy Ádám / Front-end tesztelések (pl.: MP4 lejátszása menübe), tanulás, front-end. - Szabó Attila, Varsa Laci.</t>
     </r>
   </si>
 </sst>
@@ -355,7 +496,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -410,6 +551,14 @@
       <b/>
       <sz val="10"/>
       <color theme="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
@@ -966,10 +1115,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:E18"/>
+  <dimension ref="B1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1087,86 +1236,114 @@
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="3"/>
+      <c r="D12" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="17"/>
     </row>
     <row r="13" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="21"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="21"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="2:5" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="22"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="3"/>
     </row>
+    <row r="19" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="C4:C7"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="C12:C15"/>
     <mergeCell ref="B8:B11"/>
     <mergeCell ref="C8:C11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1" xr:uid="{0C6D9F65-035A-46DB-BD55-C1313CA33086}"/>
     <hyperlink ref="E5" r:id="rId2" xr:uid="{DFAAE7C7-9BD2-43F8-BD93-C95F32B8D375}"/>
-    <hyperlink ref="E8" r:id="rId3" xr:uid="{EA3C2F54-E0E3-4945-B052-D12A66D9CA56}"/>
+    <hyperlink ref="E8" r:id="rId3" xr:uid="{A67EA07D-36AA-4716-B76B-BBD3D16FF2CE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>

</xml_diff>